<commit_message>
updated the Scrum file for sprint 2 with a better plan
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66C642E-D333-4F37-BA8D-6A7F76526502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62216015-767B-4A5B-8ADD-853D69E6D90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="178">
   <si>
     <t>Product Name:</t>
   </si>
@@ -561,6 +561,21 @@
   </si>
   <si>
     <t>Not Started</t>
+  </si>
+  <si>
+    <t>Make a package to hold P05 code</t>
+  </si>
+  <si>
+    <t>Create the graphics interface with interactivity</t>
+  </si>
+  <si>
+    <t>Add interactivity to the interface through listeners</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test the user interface to make sure that it works</t>
+  </si>
+  <si>
+    <t>Push the files to Github</t>
   </si>
 </sst>
 </file>
@@ -571,7 +586,7 @@
     <numFmt numFmtId="164" formatCode="mmm\ dd"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -634,6 +649,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -721,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -851,6 +873,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1685,28 +1710,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3747,8 +3772,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5692,7 +5717,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -6947,8 +6972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -7053,7 +7078,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -7068,7 +7093,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -7086,7 +7111,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -7104,7 +7129,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -7122,7 +7147,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7140,7 +7165,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7158,7 +7183,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7176,7 +7201,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -7222,9 +7247,13 @@
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="36"/>
+      <c r="D17" s="48" t="s">
+        <v>173</v>
+      </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38"/>
     </row>
@@ -7232,9 +7261,13 @@
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="35" t="s">
+        <v>49</v>
+      </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="39"/>
+      <c r="D18" s="39" t="s">
+        <v>174</v>
+      </c>
       <c r="E18" s="37"/>
       <c r="F18" s="38"/>
     </row>
@@ -7242,9 +7275,13 @@
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="35" t="s">
+        <v>49</v>
+      </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="39" t="s">
+        <v>175</v>
+      </c>
       <c r="E19" s="37"/>
       <c r="F19" s="38"/>
     </row>
@@ -7252,9 +7289,13 @@
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>49</v>
+      </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="39"/>
+      <c r="D20" s="39" t="s">
+        <v>176</v>
+      </c>
       <c r="E20" s="37"/>
       <c r="F20" s="38"/>
     </row>
@@ -7262,9 +7303,13 @@
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="35" t="s">
+        <v>49</v>
+      </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="39"/>
+      <c r="D21" s="39" t="s">
+        <v>177</v>
+      </c>
       <c r="E21" s="37"/>
       <c r="F21" s="38"/>
     </row>

</xml_diff>

<commit_message>
updated Scrum_Sprint_2 for finished store package
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62216015-767B-4A5B-8ADD-853D69E6D90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C834FBB5-992A-4347-8D2D-3605575C62A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="179">
   <si>
     <t>Product Name:</t>
   </si>
@@ -566,9 +566,6 @@
     <t>Make a package to hold P05 code</t>
   </si>
   <si>
-    <t>Create the graphics interface with interactivity</t>
-  </si>
-  <si>
     <t>Add interactivity to the interface through listeners</t>
   </si>
   <si>
@@ -576,6 +573,12 @@
   </si>
   <si>
     <t>Push the files to Github</t>
+  </si>
+  <si>
+    <t>Completed Day 1</t>
+  </si>
+  <si>
+    <t>Create the graphics interface without interactivity</t>
   </si>
 </sst>
 </file>
@@ -859,6 +862,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -873,9 +879,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1713,25 +1716,25 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3796,12 +3799,12 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
@@ -3812,12 +3815,12 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3856,60 +3859,60 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A6"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A7"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A8"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A9"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
@@ -4137,10 +4140,10 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="44" t="s">
+      <c r="F22" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="45"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13" t="s">
         <v>19</v>
@@ -6972,8 +6975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -7093,11 +7096,11 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -7111,7 +7114,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -7129,7 +7132,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -7147,7 +7150,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7165,7 +7168,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7183,7 +7186,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7201,7 +7204,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -7251,10 +7254,12 @@
         <v>46</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -7266,7 +7271,7 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="39" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="38"/>
@@ -7280,7 +7285,7 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="38"/>
@@ -7294,7 +7299,7 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="38"/>
@@ -7308,7 +7313,7 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E21" s="37"/>
       <c r="F21" s="38"/>

</xml_diff>

<commit_message>
Updated Scrum file for Sprint 3
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF98528C-7CBB-49CB-B122-5624A4742DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61C0E0B-C5CA-431A-B991-9F9C73194804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="196">
   <si>
     <t>Product Name:</t>
   </si>
@@ -597,6 +597,39 @@
   </si>
   <si>
     <t>I made my own icons so there is not credits for those</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a save method </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Create a constructor that reads in data</t>
+  </si>
+  <si>
+    <t>Push customer to github</t>
+  </si>
+  <si>
+    <t>Push option to github</t>
+  </si>
+  <si>
+    <t>Push Computer to github</t>
+  </si>
+  <si>
+    <t>Make a new logo for the company</t>
+  </si>
+  <si>
+    <t>Add functionality to save data through the GUI</t>
+  </si>
+  <si>
+    <t>Add functionality to create a new store through the GUI</t>
+  </si>
+  <si>
+    <t>Add functionality to save data to a different file through GUI</t>
+  </si>
+  <si>
+    <t>Add functionality to load saved data through the GUI</t>
   </si>
 </sst>
 </file>
@@ -1126,13 +1159,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2045,28 +2078,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3338,7 +3371,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>523162</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
@@ -3793,8 +3826,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -4042,11 +4075,11 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="5"/>
@@ -4066,7 +4099,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4086,7 +4119,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4477,7 +4510,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="H32" s="18" t="s">
         <v>31</v>
@@ -4603,8 +4636,12 @@
       <c r="E36" s="16">
         <v>5</v>
       </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
+      <c r="F36" s="17">
+        <v>3</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="H36" s="18" t="s">
         <v>70</v>
       </c>
@@ -4632,8 +4669,12 @@
       <c r="E37" s="16">
         <v>13</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
+      <c r="F37" s="17">
+        <v>3</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="H37" s="18" t="s">
         <v>79</v>
       </c>
@@ -4661,8 +4702,12 @@
       <c r="E38" s="16">
         <v>1</v>
       </c>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
+      <c r="F38" s="17">
+        <v>3</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="H38" s="18" t="s">
         <v>79</v>
       </c>
@@ -4690,8 +4735,12 @@
       <c r="E39" s="16">
         <v>5</v>
       </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
+      <c r="F39" s="17">
+        <v>3</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="H39" s="18" t="s">
         <v>79</v>
       </c>
@@ -4719,8 +4768,12 @@
       <c r="E40" s="16">
         <v>8</v>
       </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
+      <c r="F40" s="17">
+        <v>3</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="H40" s="18" t="s">
         <v>79</v>
       </c>
@@ -5722,7 +5775,7 @@
       <formula1>"1,2,3,4"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank initially (hint: Use the Delete key)_x000a_Select &quot;In Work&quot; when you begin designing and coding this feature._x000a_Select &quot;In Test&quot; when this feature is fully coded and you are testing it._x000a_Select  Finished ONLY when the feature works well and is READY TO" sqref="G24:G100" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank initially (hint: Use the Delete key)_x000a_Select &quot;In Work&quot; when you begin designing and coding this feature._x000a_Select &quot;In Test&quot; when this feature is fully coded and you are testing it._x000a_Select  Finished ONLY when the feature works well and is READY TO" sqref="G41:G100 G24:G39" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"Not Started,In Work,In Test,Finished in Sprint 1,Finished in Sprint 2,Finished in Sprint 3,Finished in Sprint 4,Finished in Sprint 5,Finished in Sprint 6"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5741,8 +5794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -6997,8 +7050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="B13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -8211,8 +8264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -8317,7 +8370,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -8332,7 +8385,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8350,7 +8403,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8368,7 +8421,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8386,7 +8439,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -8404,7 +8457,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -8422,7 +8475,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8440,7 +8493,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8486,142 +8539,224 @@
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="E17" s="37"/>
+      <c r="D17" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="37"/>
+      <c r="D18" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="37"/>
+      <c r="D19" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F19" s="38"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="37"/>
+      <c r="D20" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="37"/>
+      <c r="D21" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37"/>
+      <c r="D22" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F22" s="38"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37"/>
+      <c r="D23" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
+      <c r="D24" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
+      <c r="D25" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>10</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="37"/>
+      <c r="D26" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F26" s="38"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>11</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="35" t="s">
+        <v>78</v>
+      </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="37"/>
+      <c r="D27" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>12</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="37"/>
+      <c r="D28" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>13</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="39" t="s">
+        <v>87</v>
+      </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="37"/>
+      <c r="D29" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F29" s="38"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>14</v>
       </c>
-      <c r="B30" s="35"/>
+      <c r="B30" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="37"/>
+      <c r="D30" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>177</v>
+      </c>
       <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -9330,7 +9465,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D100" xr:uid="{00000000-0002-0000-0300-000003000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D19 D21:D22 D24:D100" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9344,12 +9479,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -9369,7 +9504,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17:B100</xm:sqref>
+          <xm:sqref>B26:B28 B31:B100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
updated Scrum spreadsheet for alot of stuff
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61C0E0B-C5CA-431A-B991-9F9C73194804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86CC266-A307-48D7-A2E4-D528A3DEF8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="198">
   <si>
     <t>Product Name:</t>
   </si>
@@ -602,9 +602,6 @@
     <t>Finished in Sprint 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Create a save method </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Create a constructor that reads in data</t>
   </si>
   <si>
@@ -620,16 +617,25 @@
     <t>Make a new logo for the company</t>
   </si>
   <si>
-    <t>Add functionality to save data through the GUI</t>
-  </si>
-  <si>
     <t>Add functionality to create a new store through the GUI</t>
   </si>
   <si>
-    <t>Add functionality to save data to a different file through GUI</t>
-  </si>
-  <si>
     <t>Add functionality to load saved data through the GUI</t>
+  </si>
+  <si>
+    <t>Create a save method for customer</t>
+  </si>
+  <si>
+    <t>Create a save method for option</t>
+  </si>
+  <si>
+    <t>Create a save method for computer</t>
+  </si>
+  <si>
+    <t>Add functionality to save data to a default file through the GUI</t>
+  </si>
+  <si>
+    <t>Add functionality to save data to a specified file through the GUI</t>
   </si>
 </sst>
 </file>
@@ -1159,13 +1165,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2084,22 +2090,22 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3826,7 +3832,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
@@ -4075,11 +4081,11 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="5"/>
@@ -4099,7 +4105,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4119,7 +4125,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4673,7 +4679,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="H37" s="18" t="s">
         <v>79</v>
@@ -4739,7 +4745,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="H39" s="18" t="s">
         <v>79</v>
@@ -4772,7 +4778,7 @@
         <v>3</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="H40" s="18" t="s">
         <v>79</v>
@@ -8264,8 +8270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -8388,7 +8394,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
+        <f>COUNTIF(E$20:E$995, "Completed Day 1")</f>
         <v>0</v>
       </c>
       <c r="D8" s="25"/>
@@ -8403,11 +8409,11 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C9" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <f>COUNTIF(E$20:E$995, "Completed Day 2")</f>
+        <v>6</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -8421,11 +8427,11 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C10" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>0</v>
+        <f>COUNTIF(E$20:E$995, "Completed Day 3")</f>
+        <v>2</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -8439,11 +8445,11 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C11" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>0</v>
+        <f>COUNTIF(E$20:E$995, "Completed Day 4")</f>
+        <v>1</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -8457,10 +8463,10 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C12" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
+        <f>COUNTIF(E$20:E$995, "Completed Day 5")</f>
         <v>0</v>
       </c>
       <c r="D12" s="25"/>
@@ -8475,10 +8481,10 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C13" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
+        <f>COUNTIF(E$20:E$995, "Completed Day 6")</f>
         <v>0</v>
       </c>
       <c r="D13" s="25"/>
@@ -8493,10 +8499,10 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C14" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
+        <f>COUNTIF(E$20:E$995, "Completed Day 7")</f>
         <v>0</v>
       </c>
       <c r="D14" s="25"/>
@@ -8544,10 +8550,10 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="43" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F17" s="38"/>
     </row>
@@ -8560,10 +8566,10 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F18" s="38"/>
     </row>
@@ -8576,10 +8582,10 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F19" s="38"/>
     </row>
@@ -8592,10 +8598,10 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="43" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F20" s="38"/>
     </row>
@@ -8608,10 +8614,10 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F21" s="38"/>
     </row>
@@ -8624,10 +8630,10 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F22" s="38"/>
     </row>
@@ -8640,10 +8646,10 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="43" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F23" s="38"/>
     </row>
@@ -8656,10 +8662,10 @@
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F24" s="38"/>
     </row>
@@ -8672,10 +8678,10 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F25" s="38"/>
     </row>
@@ -8688,7 +8694,7 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>177</v>
@@ -8704,10 +8710,10 @@
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="39" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="F27" s="38"/>
     </row>
@@ -8720,14 +8726,14 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="39" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E28" s="37" t="s">
         <v>177</v>
       </c>
       <c r="F28" s="38"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>13</v>
       </c>
@@ -8736,10 +8742,10 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="39" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="F29" s="38"/>
     </row>
@@ -8752,10 +8758,10 @@
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="39" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="F30" s="38"/>
     </row>
@@ -9469,12 +9475,12 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0300-000005000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0300-000004000000}">
       <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0300-000005000000}">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>